<commit_message>
Update translations and add kendo filter messages
</commit_message>
<xml_diff>
--- a/TRANS_Japanese Translation-ECOS-MAPS.xlsx
+++ b/TRANS_Japanese Translation-ECOS-MAPS.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="1515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2387" uniqueCount="1521">
   <si>
     <t>No frames selected</t>
   </si>
@@ -4917,6 +4917,87 @@
     <t>重複データの処理中…</t>
   </si>
   <si>
+    <t>ページあたりの表示件数</t>
+  </si>
+  <si>
+    <t>表示するアイテムがありません</t>
+  </si>
+  <si>
+    <t>変更内容は保存されません。続けますか？</t>
+  </si>
+  <si>
+    <t xml:space="preserve">全%{total} 件中%{x} - %{y} </t>
+  </si>
+  <si>
+    <t>ホーム</t>
+  </si>
+  <si>
+    <t>ファイルの処理中にエラーが発生しました。はじめからやりなおしてください</t>
+  </si>
+  <si>
+    <t>登録媒体の絞込み</t>
+  </si>
+  <si>
+    <t>ファイルを選ぶ</t>
+  </si>
+  <si>
+    <t>ファイルのアップロード</t>
+  </si>
+  <si>
+    <t>再読み込み中…</t>
+  </si>
+  <si>
+    <t>絞込み検索</t>
+  </si>
+  <si>
+    <t>マッピングされていません</t>
+  </si>
+  <si>
+    <t>ja (JAPANESE) [Received on Fri 16/10/2015 16:16]</t>
+  </si>
+  <si>
+    <t>媒体 %{count} 個が追加されました</t>
+  </si>
+  <si>
+    <t>%{count} POIが追加されました</t>
+  </si>
+  <si>
+    <t>Shape %{count} 個が追加されました</t>
+  </si>
+  <si>
+    <t>次の媒体を取得:  %{name}</t>
+  </si>
+  <si>
+    <t>MSG_I_OpeningMapPleaseWait</t>
+  </si>
+  <si>
+    <t>%{tabName} タブを%ローディング中　</t>
+  </si>
+  <si>
+    <t>Shapeから媒体を{count}%取得中</t>
+  </si>
+  <si>
+    <t>媒体ID</t>
+  </si>
+  <si>
+    <t>LBL_Complete</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>完全な</t>
+  </si>
+  <si>
+    <t>LBL_Deleted</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>削除されました</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -4936,71 +5017,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: %{count} / {total}</t>
+      <t>: %{count} / %{total}</t>
     </r>
-  </si>
-  <si>
-    <t>ページあたりの表示件数</t>
-  </si>
-  <si>
-    <t>表示するアイテムがありません</t>
-  </si>
-  <si>
-    <t>変更内容は保存されません。続けますか？</t>
-  </si>
-  <si>
-    <t xml:space="preserve">全%{total} 件中%{x} - %{y} </t>
-  </si>
-  <si>
-    <t>ホーム</t>
-  </si>
-  <si>
-    <t>ファイルの処理中にエラーが発生しました。はじめからやりなおしてください</t>
-  </si>
-  <si>
-    <t>登録媒体の絞込み</t>
-  </si>
-  <si>
-    <t>ファイルを選ぶ</t>
-  </si>
-  <si>
-    <t>ファイルのアップロード</t>
-  </si>
-  <si>
-    <t>再読み込み中…</t>
-  </si>
-  <si>
-    <t>絞込み検索</t>
-  </si>
-  <si>
-    <t>マッピングされていません</t>
-  </si>
-  <si>
-    <t>ja (JAPANESE) [Received on Fri 16/10/2015 16:16]</t>
-  </si>
-  <si>
-    <t>媒体 %{count} 個が追加されました</t>
-  </si>
-  <si>
-    <t>%{count} POIが追加されました</t>
-  </si>
-  <si>
-    <t>Shape %{count} 個が追加されました</t>
-  </si>
-  <si>
-    <t>次の媒体を取得:  %{name}</t>
-  </si>
-  <si>
-    <t>MSG_I_OpeningMapPleaseWait</t>
-  </si>
-  <si>
-    <t>%{tabName} タブを%ローディング中　</t>
-  </si>
-  <si>
-    <t>Shapeから媒体を{count}%取得中</t>
-  </si>
-  <si>
-    <t>媒体ID</t>
   </si>
 </sst>
 </file>
@@ -5697,10 +5715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F398"/>
+  <dimension ref="A1:F401"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E363" workbookViewId="0">
+      <selection activeCell="F384" sqref="F384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5729,7 +5747,7 @@
         <v>434</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -10469,7 +10487,7 @@
         <v>1218</v>
       </c>
       <c r="F238" s="22" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="239" spans="1:6">
@@ -10489,7 +10507,7 @@
         <v>1219</v>
       </c>
       <c r="F239" s="22" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -10509,7 +10527,7 @@
         <v>1218</v>
       </c>
       <c r="F240" s="22" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="241" spans="1:6">
@@ -12617,7 +12635,7 @@
         <v>239</v>
       </c>
       <c r="B346" s="11" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C346" s="11" t="s">
         <v>845</v>
@@ -13189,7 +13207,7 @@
         <v>1208</v>
       </c>
       <c r="F374" s="11" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="375" spans="1:6">
@@ -13209,7 +13227,7 @@
         <v>1209</v>
       </c>
       <c r="F375" s="11" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="376" spans="1:6">
@@ -13229,7 +13247,7 @@
         <v>1210</v>
       </c>
       <c r="F376" s="11" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="377" spans="1:6">
@@ -13376,7 +13394,7 @@
         <v>1261</v>
       </c>
       <c r="F384" s="29" t="s">
-        <v>1493</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="385" spans="1:6">
@@ -13396,7 +13414,7 @@
         <v>1270</v>
       </c>
       <c r="F385" s="30" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="386" spans="1:6">
@@ -13416,7 +13434,7 @@
         <v>1271</v>
       </c>
       <c r="F386" s="30" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="387" spans="1:6" s="13" customFormat="1">
@@ -13436,7 +13454,7 @@
         <v>1275</v>
       </c>
       <c r="F387" s="26" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="388" spans="1:6">
@@ -13456,7 +13474,7 @@
         <v>1279</v>
       </c>
       <c r="F388" s="31" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="389" spans="1:6">
@@ -13476,7 +13494,7 @@
         <v>1281</v>
       </c>
       <c r="F389" s="28" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="390" spans="1:6">
@@ -13496,7 +13514,7 @@
         <v>1284</v>
       </c>
       <c r="F390" s="28" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="391" spans="1:6">
@@ -13516,7 +13534,7 @@
         <v>1287</v>
       </c>
       <c r="F391" s="27" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="392" spans="1:6">
@@ -13536,7 +13554,7 @@
         <v>1291</v>
       </c>
       <c r="F392" s="32" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="393" spans="1:6">
@@ -13556,7 +13574,7 @@
         <v>1294</v>
       </c>
       <c r="F393" s="33" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="394" spans="1:6">
@@ -13576,7 +13594,7 @@
         <v>1297</v>
       </c>
       <c r="F394" s="32" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="395" spans="1:6">
@@ -13596,7 +13614,7 @@
         <v>1299</v>
       </c>
       <c r="F395" s="32" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="396" spans="1:6">
@@ -13616,7 +13634,7 @@
         <v>1302</v>
       </c>
       <c r="F396" s="32" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="398" spans="1:6">
@@ -13636,7 +13654,51 @@
         <v>1304</v>
       </c>
       <c r="F398" s="15" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6">
+      <c r="E399" s="15"/>
+      <c r="F399" s="15"/>
+    </row>
+    <row r="400" spans="1:6">
+      <c r="A400" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B400" s="11" t="s">
         <v>1514</v>
+      </c>
+      <c r="C400" s="11" t="s">
+        <v>1514</v>
+      </c>
+      <c r="D400" s="11" t="s">
+        <v>1515</v>
+      </c>
+      <c r="E400" s="9" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F400" s="11" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6">
+      <c r="A401" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B401" s="11" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C401" s="11" t="s">
+        <v>1517</v>
+      </c>
+      <c r="D401" s="11" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E401" s="9" t="s">
+        <v>1519</v>
+      </c>
+      <c r="F401" s="11" t="s">
+        <v>1519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>